<commit_message>
add env var and copy for results
</commit_message>
<xml_diff>
--- a/sample_sheet.xlsx
+++ b/sample_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/tkartzin/tdivoll/obitools2-pipeline/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdivoll/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6492406-065D-EE45-AC23-3273D15761EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3409606E-34DD-6948-BE1E-A6A4F9CF2275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6820" yWindow="1720" windowWidth="34480" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1720" windowWidth="30240" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,19 +187,26 @@
     <t>Folder</t>
   </si>
   <si>
-    <t>URI_1</t>
-  </si>
-  <si>
-    <t>URI_2</t>
+    <t>URI_20221013</t>
+  </si>
+  <si>
+    <t>URI_20230519</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -220,21 +227,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -250,7 +245,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,12 +255,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -303,36 +292,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,18 +640,19 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:L13"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="8" customWidth="1"/>
-    <col min="11" max="12" width="12.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="12.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="11" customWidth="1"/>
+    <col min="11" max="12" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -706,499 +697,499 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="12">
+      <c r="J2" s="7">
         <v>20220725</v>
       </c>
-      <c r="K2" s="12">
+      <c r="K2" s="7">
         <v>20220805</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <v>20221013</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="7">
         <v>20220725</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="7">
         <v>20220805</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>20221013</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="7">
         <v>20220725</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="7">
         <v>20220805</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>20221013</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="9">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>20220801</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>20220810</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <v>20221013</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="9">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>20220801</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>20220810</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
         <v>20221013</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="9">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>20220801</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>20220810</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <v>20221013</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
         <v>1</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="7">
         <v>20231201</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="7">
         <v>20230422</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="5">
         <v>20230519</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
         <v>1</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="7">
         <v>20231201</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="7">
         <v>20230422</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <v>20230519</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
         <v>1</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="7">
         <v>20231201</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="7">
         <v>20230422</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="5">
         <v>20230519</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
         <v>1</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="7">
         <v>20231201</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="7">
         <v>20230422</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="5">
         <v>20230519</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
         <v>1</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="7">
         <v>20231202</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="7">
         <v>20230422</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="5">
         <v>20230519</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
         <v>1</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="7">
         <v>20231203</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="7">
         <v>20230422</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="5">
         <v>20230519</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="13" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="C10:C13">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF($A:$AH, INDIRECT(ADDRESS(ROW(), COLUMN(),)))&gt;1</formula>

</xml_diff>